<commit_message>
Add space to string.replace"&"
</commit_message>
<xml_diff>
--- a/CLIMB clery charts.xlsx
+++ b/CLIMB clery charts.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Clery charts - all\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshua.boyan\Desktop\excel-to-html-table\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12885" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12885"/>
   </bookViews>
   <sheets>
     <sheet name="CLIMB Criminal Offenses" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="27">
   <si>
     <t>Arson</t>
   </si>
@@ -76,9 +76,6 @@
     <t>Criminal Offenses</t>
   </si>
   <si>
-    <t>CLIMB</t>
-  </si>
-  <si>
     <t>Stalking</t>
   </si>
   <si>
@@ -107,6 +104,9 @@
   </si>
   <si>
     <t>Arrests &amp; Diciplinary Actions</t>
+  </si>
+  <si>
+    <t>&amp;nbsp;</t>
   </si>
 </sst>
 </file>
@@ -217,7 +217,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -225,9 +225,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -521,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,56 +530,70 @@
     <col min="2" max="7" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="7"/>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
+      <c r="A2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="2">
+        <v>2013</v>
+      </c>
+      <c r="C2" s="2">
+        <v>2014</v>
+      </c>
+      <c r="D2" s="2">
+        <v>2015</v>
+      </c>
+      <c r="E2" s="2">
+        <v>2013</v>
+      </c>
+      <c r="F2" s="2">
+        <v>2014</v>
+      </c>
+      <c r="G2" s="2">
+        <v>2015</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
+      <c r="A3" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="B3" s="2">
-        <v>2013</v>
+        <v>0</v>
       </c>
       <c r="C3" s="2">
-        <v>2014</v>
+        <v>0</v>
       </c>
       <c r="D3" s="2">
-        <v>2015</v>
+        <v>0</v>
       </c>
       <c r="E3" s="2">
-        <v>2013</v>
+        <v>0</v>
       </c>
       <c r="F3" s="2">
-        <v>2014</v>
+        <v>0</v>
       </c>
       <c r="G3" s="2">
-        <v>2015</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>12</v>
+      <c r="A4" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="B4" s="2">
         <v>0</v>
@@ -605,54 +616,66 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2">
         <v>0</v>
       </c>
-      <c r="C5" s="2">
-        <v>0</v>
-      </c>
-      <c r="D5" s="2">
-        <v>0</v>
+      <c r="C5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="E5" s="2">
         <v>0</v>
       </c>
-      <c r="F5" s="2">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2">
-        <v>0</v>
+      <c r="F5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="2">
-        <v>0</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="2"/>
+        <v>8</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="C7" s="2">
         <v>0</v>
       </c>
       <c r="D7" s="2">
         <v>0</v>
       </c>
-      <c r="E7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="F7" s="2">
         <v>0</v>
       </c>
@@ -662,50 +685,66 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2">
-        <v>0</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2">
-        <v>0</v>
-      </c>
-      <c r="G8" s="2">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="2">
-        <v>0</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2">
-        <v>0</v>
-      </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="C10" s="2">
         <v>0</v>
       </c>
       <c r="D10" s="2">
         <v>0</v>
       </c>
-      <c r="E10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="F10" s="2">
         <v>0</v>
       </c>
@@ -715,16 +754,20 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0</v>
+      </c>
       <c r="C11" s="2">
         <v>0</v>
       </c>
       <c r="D11" s="2">
         <v>0</v>
       </c>
-      <c r="E11" s="2"/>
+      <c r="E11" s="2">
+        <v>0</v>
+      </c>
       <c r="F11" s="2">
         <v>0</v>
       </c>
@@ -734,7 +777,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B12" s="2">
         <v>0</v>
@@ -757,7 +800,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B13" s="2">
         <v>0</v>
@@ -780,7 +823,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B14" s="2">
         <v>0</v>
@@ -798,12 +841,12 @@
         <v>0</v>
       </c>
       <c r="G14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B15" s="2">
         <v>0</v>
@@ -821,48 +864,25 @@
         <v>0</v>
       </c>
       <c r="G15" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" s="2">
-        <v>0</v>
-      </c>
-      <c r="C16" s="2">
-        <v>0</v>
-      </c>
-      <c r="D16" s="2">
-        <v>0</v>
-      </c>
-      <c r="E16" s="2">
-        <v>0</v>
-      </c>
-      <c r="F16" s="2">
-        <v>0</v>
-      </c>
-      <c r="G16" s="2">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="A1:G1"/>
+  <mergeCells count="2">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,56 +891,68 @@
     <col min="2" max="7" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="7"/>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2">
+        <v>2013</v>
+      </c>
+      <c r="C2" s="2">
+        <v>2014</v>
+      </c>
+      <c r="D2" s="2">
+        <v>2015</v>
+      </c>
+      <c r="E2" s="2">
+        <v>2013</v>
+      </c>
+      <c r="F2" s="2">
+        <v>2014</v>
+      </c>
+      <c r="G2" s="2">
+        <v>2015</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
+      <c r="A3" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="B3" s="2">
-        <v>2013</v>
+        <v>0</v>
       </c>
       <c r="C3" s="2">
-        <v>2014</v>
+        <v>0</v>
       </c>
       <c r="D3" s="2">
-        <v>2015</v>
+        <v>0</v>
       </c>
       <c r="E3" s="2">
-        <v>2013</v>
+        <v>0</v>
       </c>
       <c r="F3" s="2">
-        <v>2014</v>
+        <v>0</v>
       </c>
       <c r="G3" s="2">
-        <v>2015</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B4" s="2">
         <v>0</v>
@@ -943,7 +975,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B5" s="2">
         <v>0</v>
@@ -964,34 +996,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="2">
-        <v>0</v>
-      </c>
-      <c r="C6" s="2">
-        <v>0</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0</v>
-      </c>
-      <c r="G6" s="2">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="A1:G1"/>
+  <mergeCells count="2">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -999,10 +1007,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1011,67 +1019,79 @@
     <col min="2" max="7" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="7"/>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2">
         <v>2013</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C2" s="2">
         <v>2014</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D2" s="2">
         <v>2015</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E2" s="2">
         <v>2013</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F2" s="2">
         <v>2014</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G2" s="2">
         <v>2015</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
+    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B5" s="2">
         <v>0</v>
@@ -1094,73 +1114,73 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="9"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="2">
-        <v>0</v>
-      </c>
-      <c r="C6" s="2">
-        <v>0</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0</v>
-      </c>
-      <c r="G6" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="2">
-        <v>0</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0</v>
-      </c>
-      <c r="D7" s="2">
-        <v>0</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0</v>
-      </c>
-      <c r="F7" s="2">
-        <v>0</v>
-      </c>
-      <c r="G7" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="12"/>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
+      <c r="B9" s="2">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B10" s="2">
         <v>0</v>
@@ -1183,7 +1203,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B11" s="2">
         <v>0</v>
@@ -1204,37 +1224,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="2">
-        <v>0</v>
-      </c>
-      <c r="C12" s="2">
-        <v>0</v>
-      </c>
-      <c r="D12" s="2">
-        <v>0</v>
-      </c>
-      <c r="E12" s="2">
-        <v>0</v>
-      </c>
-      <c r="F12" s="2">
-        <v>0</v>
-      </c>
-      <c r="G12" s="2">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A9:G9"/>
-    <mergeCell ref="A1:G1"/>
+  <mergeCells count="5">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="A3:G3"/>
     <mergeCell ref="A8:G8"/>
+    <mergeCell ref="A7:G7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>